<commit_message>
PM10 results and new ADJ matrices
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deneme/Documents/ders/smart city/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD\Courses2ndTerm\BLG556E\project\air-quality-prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE0BDC9-EEFF-F043-88A9-5061A8D7C8A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B59D962-251C-4F77-A2C2-57902F353542}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{8F870A8A-DB82-0D45-9C43-DB95A8C8E75F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8F870A8A-DB82-0D45-9C43-DB95A8C8E75F}"/>
   </bookViews>
   <sheets>
-    <sheet name="GCN_LSTM" sheetId="3" r:id="rId1"/>
+    <sheet name="GCN_LSTM_PM10" sheetId="3" r:id="rId1"/>
     <sheet name="Sayfa1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>cnn lstm</t>
   </si>
@@ -103,32 +103,44 @@
     <t>Adjacency Matris Type</t>
   </si>
   <si>
-    <t>It is a matrix created with random values.</t>
-  </si>
-  <si>
-    <t>It is a matrix created by taking the population difference.</t>
-  </si>
-  <si>
-    <t>It is a matrix created by taking the difference in gas consumption.</t>
-  </si>
-  <si>
-    <t>It is a matrix created by taking the difference in the amount of waste.</t>
-  </si>
-  <si>
-    <t>It is a matrix created by taking the distance difference between the sensors.</t>
-  </si>
-  <si>
-    <t>It is a matrix created by taking the difference in the number of parks.</t>
-  </si>
-  <si>
-    <t>Description</t>
+    <t>Waste Facilities</t>
+  </si>
+  <si>
+    <t>Uniform random values between [0, 1].</t>
+  </si>
+  <si>
+    <t>Population difference across disctricts.</t>
+  </si>
+  <si>
+    <t>Difference in gas consumption.</t>
+  </si>
+  <si>
+    <t>Value Description</t>
+  </si>
+  <si>
+    <t>Difference in the amount of produced waste.</t>
+  </si>
+  <si>
+    <t>Euclidean distance difference between the sensors.</t>
+  </si>
+  <si>
+    <t>Difference in the number of parks located around the sensors.</t>
+  </si>
+  <si>
+    <t>Inverse of the total distance between a sensor and all waste facilities.</t>
+  </si>
+  <si>
+    <t>Pollution</t>
+  </si>
+  <si>
+    <t>Difference in common pollution production.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -159,6 +171,24 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -218,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -226,6 +256,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -235,16 +274,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -253,16 +286,16 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <i/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -301,20 +334,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CDAFAB6C-CFEA-BC4F-8C33-6CBD4220ABAA}" name="Tablo13" displayName="Tablo13" ref="A1:D7" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D7" xr:uid="{47CC033D-BE82-E048-972C-A6CD74CE746C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CDAFAB6C-CFEA-BC4F-8C33-6CBD4220ABAA}" name="Tablo13" displayName="Tablo13" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D9" xr:uid="{47CC033D-BE82-E048-972C-A6CD74CE746C}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{BCEDA02B-B4FB-0946-9F40-8486D6856A6E}" name="Adjacency Matris Type" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{22890D4D-255E-4F47-864E-5CD826702D4E}" name="MSE" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{4DB438A8-39F9-574D-9CC9-ADA92E6CCBC8}" name="RMSE" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{63F9D63A-1280-7E4A-AC53-46479D817594}" name="Description" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{4DB438A8-39F9-574D-9CC9-ADA92E6CCBC8}" name="RMSE" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{63F9D63A-1280-7E4A-AC53-46479D817594}" name="Value Description" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -610,96 +643,149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9BF5BF4-2C7A-D644-B2C5-317E818EF65A}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="63.83203125" customWidth="1"/>
+    <col min="4" max="4" width="63.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="7">
+        <v>635.27724244512399</v>
+      </c>
+      <c r="C2" s="7">
+        <v>25.2047067518176</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="7">
+        <v>638.65099999999995</v>
+      </c>
+      <c r="C3" s="7">
+        <v>25.271999999999998</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="7">
+        <v>657.66272691585402</v>
+      </c>
+      <c r="C4" s="7">
+        <v>25.644935697245401</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="7">
+        <v>633.029</v>
+      </c>
+      <c r="C5" s="7">
+        <v>25.16</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="7">
+        <v>647.49599999999998</v>
+      </c>
+      <c r="C6" s="7">
+        <v>25.446000000000002</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="13" t="s">
+    <row r="7" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="7">
+        <v>607.89800000000002</v>
+      </c>
+      <c r="C7" s="7">
+        <v>24.655999999999999</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="13" t="s">
-        <v>30</v>
+      <c r="B8" s="7">
+        <v>615.83057262393595</v>
+      </c>
+      <c r="C8" s="7">
+        <v>24.815933845494001</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="7">
+        <v>638.18499999999995</v>
+      </c>
+      <c r="C9" s="7">
+        <v>25.262</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -712,41 +798,41 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="7" t="s">
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8" t="s">
+      <c r="G2" s="11"/>
+      <c r="H2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -775,7 +861,7 @@
         <v>12.63</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -804,7 +890,7 @@
         <v>9.36</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -833,7 +919,7 @@
         <v>8.84</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -862,7 +948,7 @@
         <v>5.56</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -891,7 +977,7 @@
         <v>59.05</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -920,7 +1006,7 @@
         <v>15.99</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -949,7 +1035,7 @@
         <v>7.97</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -978,7 +1064,7 @@
         <v>15.32</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1007,7 +1093,7 @@
         <v>15.22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1036,7 +1122,7 @@
         <v>16.23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1073,7 +1159,7 @@
         <v>16.616999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
results of pollution and meteology data
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD\Courses2ndTerm\BLG556E\project\air-quality-prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deneme/Documents/ders/smart city/project/air-quality-prediction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148F91ED-EBE6-4354-BC00-41297E2C7DE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1322515-9434-4F40-BFE3-2E1236BFE573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8F870A8A-DB82-0D45-9C43-DB95A8C8E75F}"/>
+    <workbookView xWindow="-2360" yWindow="-20000" windowWidth="33600" windowHeight="19120" activeTab="1" xr2:uid="{8F870A8A-DB82-0D45-9C43-DB95A8C8E75F}"/>
   </bookViews>
   <sheets>
     <sheet name="GCN_LSTM_PM10" sheetId="3" r:id="rId1"/>
-    <sheet name="Sayfa1" sheetId="1" r:id="rId2"/>
+    <sheet name="LSTM" sheetId="6" r:id="rId2"/>
+    <sheet name="old_workbook" sheetId="5" r:id="rId3"/>
+    <sheet name="old_workbook_1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="60">
   <si>
     <t>cnn lstm</t>
   </si>
@@ -146,13 +148,73 @@
   </si>
   <si>
     <t>Difference in the number of neighboors reported by IBB.</t>
+  </si>
+  <si>
+    <t>All Pollutants</t>
+  </si>
+  <si>
+    <t>Average humidity (% RH) measured from the respective sensor in the given hour.</t>
+  </si>
+  <si>
+    <t>Average wind direction (km / h) measured from the respective sensor at the given hour.</t>
+  </si>
+  <si>
+    <t>Average amount of precipitation (kg / m²) measured from the relevant sensor in the given hour.</t>
+  </si>
+  <si>
+    <t>Average road temperature (&amp; ordm; C) measured from the respective sensor at the given hour.</t>
+  </si>
+  <si>
+    <t>Multivariate Type</t>
+  </si>
+  <si>
+    <t>Average Humidity</t>
+  </si>
+  <si>
+    <t>Average Wind</t>
+  </si>
+  <si>
+    <t>Average Temperature</t>
+  </si>
+  <si>
+    <t>Average Direction Of Wind</t>
+  </si>
+  <si>
+    <t>Average Precipitation</t>
+  </si>
+  <si>
+    <t>Average Road Temperature</t>
+  </si>
+  <si>
+    <t>All pollution values PM10 ( µg/m3 ), SO2 ( µg/m3 ), CO ( µg/m3 ), NO2 ( µg/m3 ), NOX ( µg/m3 ), O3 ( µg/m3 ), PM 2.5 ( µg/m3 )</t>
+  </si>
+  <si>
+    <t>All Pollutants &amp; All Meteorology</t>
+  </si>
+  <si>
+    <t>All Meteorology</t>
+  </si>
+  <si>
+    <t>All meteorology data (OBSERVATORY_NAME, AVERAGE_TEMPERATURE, AVERAGE_HUMIDITY, AVERAGE_WIND, AVERAGE_DIRECTIONOFWIND, AVERAGE_PRECIPITATION, AVERAGE_ROAD_TEMPERATURE)</t>
+  </si>
+  <si>
+    <t>All pollution values PM10 ( µg/m3 ), SO2 ( µg/m3 ), CO ( µg/m3 ), NO2 ( µg/m3 ), NOX ( µg/m3 ), O3 ( µg/m3 ), PM 2.5 ( µg/m3 ) &amp; All meteorology data (OBSERVATORY_NAME, AVERAGE_TEMPERATURE, AVERAGE_HUMIDITY, AVERAGE_WIND, AVERAGE_DIRECTIONOFWIND, AVERAGE_PRECIPITATION, AVERAGE_ROAD_TEMPERATURE)</t>
+  </si>
+  <si>
+    <t>Average temperature (&amp; ordm; C) measured from the respective sensor at the given hour.</t>
+  </si>
+  <si>
+    <t>Average wind speed (km / h) measured from the respective sensor in the given hour.</t>
+  </si>
+  <si>
+    <t>Town</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -203,8 +265,16 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,6 +290,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -260,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -292,11 +380,78 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="13">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <sz val="14"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <i/>
@@ -346,20 +501,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CDAFAB6C-CFEA-BC4F-8C33-6CBD4220ABAA}" name="Tablo13" displayName="Tablo13" ref="A1:D11" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CDAFAB6C-CFEA-BC4F-8C33-6CBD4220ABAA}" name="Tablo13" displayName="Tablo13" ref="A1:D11" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:D11" xr:uid="{47CC033D-BE82-E048-972C-A6CD74CE746C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BCEDA02B-B4FB-0946-9F40-8486D6856A6E}" name="Adjacency Matris Type" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{22890D4D-255E-4F47-864E-5CD826702D4E}" name="MSE" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{4DB438A8-39F9-574D-9CC9-ADA92E6CCBC8}" name="RMSE" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{63F9D63A-1280-7E4A-AC53-46479D817594}" name="Value Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{BCEDA02B-B4FB-0946-9F40-8486D6856A6E}" name="Adjacency Matris Type" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{22890D4D-255E-4F47-864E-5CD826702D4E}" name="MSE" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{4DB438A8-39F9-574D-9CC9-ADA92E6CCBC8}" name="RMSE" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{63F9D63A-1280-7E4A-AC53-46479D817594}" name="Value Description" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CDD45F58-BC3B-044F-A441-CADFB99042D8}" name="Tablo135" displayName="Tablo135" ref="A1:E19" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E19" xr:uid="{EE1E83D7-2F3E-6843-B7A5-BAD59CDCBE71}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{70BE4064-60C5-1C43-82A7-5D28319CE4B4}" name="Multivariate Type" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{1E92B077-F88A-7543-915C-0735A7540EB3}" name="MSE" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{EBAABF72-3ED8-444E-A2DB-7C2D20FA4524}" name="RMSE" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{641A573E-F733-8440-A0E2-5C8176298AA3}" name="Value Description" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{14BA1D5F-1C5F-494E-BDE5-C0DD6583EC6B}" name="Town" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -657,18 +826,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9BF5BF4-2C7A-D644-B2C5-317E818EF65A}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="63.875" customWidth="1"/>
+    <col min="4" max="4" width="63.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
@@ -682,7 +851,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>23</v>
       </c>
@@ -696,7 +865,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>18</v>
       </c>
@@ -710,7 +879,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>19</v>
       </c>
@@ -724,7 +893,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>20</v>
       </c>
@@ -738,7 +907,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>21</v>
       </c>
@@ -752,7 +921,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>22</v>
       </c>
@@ -766,7 +935,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>25</v>
       </c>
@@ -780,7 +949,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>34</v>
       </c>
@@ -794,7 +963,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>36</v>
       </c>
@@ -808,7 +977,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>38</v>
       </c>
@@ -832,16 +1001,637 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A48F244-53E6-1541-A02C-D5DBE0322B34}">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="132.33203125" style="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="26" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="26" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="7">
+        <v>8023</v>
+      </c>
+      <c r="C2" s="7">
+        <v>89.57</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="26" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="7">
+        <v>6369</v>
+      </c>
+      <c r="C3" s="7">
+        <v>79.8</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="26" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="7">
+        <v>5475</v>
+      </c>
+      <c r="C4" s="7">
+        <v>73.989999999999995</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="26" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="7">
+        <v>7680</v>
+      </c>
+      <c r="C5" s="7">
+        <v>87.63</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="26" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="7">
+        <v>8123</v>
+      </c>
+      <c r="C6" s="7">
+        <v>90.13</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="26" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="7">
+        <v>8141</v>
+      </c>
+      <c r="C7" s="7">
+        <v>90.23</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="26" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="7">
+        <v>8281</v>
+      </c>
+      <c r="C8" s="7">
+        <v>91</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="26" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="7">
+        <v>7887</v>
+      </c>
+      <c r="C9" s="7">
+        <v>88.81</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="26" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="7">
+        <v>8594</v>
+      </c>
+      <c r="C10" s="7">
+        <v>92.7</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="7">
+        <v>109</v>
+      </c>
+      <c r="C11" s="7">
+        <v>10.45</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="7">
+        <v>189</v>
+      </c>
+      <c r="C12" s="7">
+        <v>13.75</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="7">
+        <v>304</v>
+      </c>
+      <c r="C13" s="7">
+        <v>17.440000000000001</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="7">
+        <v>50</v>
+      </c>
+      <c r="C14" s="7">
+        <v>7</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="7">
+        <v>54</v>
+      </c>
+      <c r="C15" s="7">
+        <v>7.36</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="7">
+        <v>52</v>
+      </c>
+      <c r="C16" s="7">
+        <v>7.22</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="7">
+        <v>290</v>
+      </c>
+      <c r="C17" s="7">
+        <v>17.02</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="7">
+        <v>308</v>
+      </c>
+      <c r="C18" s="7">
+        <v>17.55</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="7">
+        <v>283</v>
+      </c>
+      <c r="C19" s="7">
+        <v>16.82</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F99379-8F87-5A43-82E5-1B393C03149F}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="159.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="21">
+        <v>50</v>
+      </c>
+      <c r="C3" s="21">
+        <v>7</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="23">
+        <v>54</v>
+      </c>
+      <c r="C4" s="23">
+        <v>7.36</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="21">
+        <v>52</v>
+      </c>
+      <c r="C5" s="21">
+        <v>7.22</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+    </row>
+    <row r="7" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="21">
+        <v>109</v>
+      </c>
+      <c r="C7" s="21">
+        <v>10.45</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="21">
+        <v>189</v>
+      </c>
+      <c r="C8" s="21">
+        <v>13.75</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="21">
+        <v>304</v>
+      </c>
+      <c r="C9" s="21">
+        <v>17.440000000000001</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+    </row>
+    <row r="11" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="24">
+        <v>8023</v>
+      </c>
+      <c r="C11" s="24">
+        <v>89.57</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="24">
+        <v>6369</v>
+      </c>
+      <c r="C12" s="24">
+        <v>79.8</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="24">
+        <v>5475</v>
+      </c>
+      <c r="C13" s="24">
+        <v>73.989999999999995</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="24">
+        <v>7680</v>
+      </c>
+      <c r="C14" s="24">
+        <v>87.63</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="24">
+        <v>8123</v>
+      </c>
+      <c r="C15" s="24">
+        <v>90.13</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="24">
+        <v>8141</v>
+      </c>
+      <c r="C16" s="24">
+        <v>90.23</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="24">
+        <v>8281</v>
+      </c>
+      <c r="C17" s="24">
+        <v>91</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="24">
+        <v>7887</v>
+      </c>
+      <c r="C18" s="24">
+        <v>88.81</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="24">
+        <v>8594</v>
+      </c>
+      <c r="C19" s="24">
+        <v>92.7</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A10:D10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D7AA4E-FDBD-DD40-8479-FB2E2AAA5078}">
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" s="14" t="s">
         <v>13</v>
       </c>
@@ -855,7 +1645,7 @@
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
@@ -873,7 +1663,7 @@
       </c>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -902,7 +1692,7 @@
         <v>12.63</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -931,7 +1721,7 @@
         <v>9.36</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -960,7 +1750,7 @@
         <v>8.84</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -989,7 +1779,7 @@
         <v>5.56</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1018,7 +1808,7 @@
         <v>59.05</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1047,7 +1837,7 @@
         <v>15.99</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1076,7 +1866,7 @@
         <v>7.97</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1105,7 +1895,7 @@
         <v>15.32</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1134,7 +1924,7 @@
         <v>15.22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1163,7 +1953,7 @@
         <v>16.23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1200,7 +1990,7 @@
         <v>16.616999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
added result of dtw method
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deneme/Documents/ders/smart city/project/air-quality-prediction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94751C9D-0F72-034D-8761-16F5FAB5F3A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED7BB3B-F782-8F4D-83FE-1D3DA733D990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="-19180" windowWidth="28640" windowHeight="17140" activeTab="1" xr2:uid="{8F870A8A-DB82-0D45-9C43-DB95A8C8E75F}"/>
+    <workbookView xWindow="640" yWindow="-18500" windowWidth="28640" windowHeight="17140" xr2:uid="{8F870A8A-DB82-0D45-9C43-DB95A8C8E75F}"/>
   </bookViews>
   <sheets>
     <sheet name="GCN_LSTM_PM10" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="66">
   <si>
     <t>cnn lstm</t>
   </si>
@@ -221,6 +221,12 @@
   </si>
   <si>
     <t>Percentage of parks over population around sensors.</t>
+  </si>
+  <si>
+    <t>Sequence Distance (Dinamic Time Warping)</t>
+  </si>
+  <si>
+    <t>Difference of sequences according to dinamic time warping formula</t>
   </si>
 </sst>
 </file>
@@ -494,6 +500,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -505,9 +514,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -588,8 +594,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CDAFAB6C-CFEA-BC4F-8C33-6CBD4220ABAA}" name="Tablo13" displayName="Tablo13" ref="A1:D13" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:D13" xr:uid="{47CC033D-BE82-E048-972C-A6CD74CE746C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CDAFAB6C-CFEA-BC4F-8C33-6CBD4220ABAA}" name="Tablo13" displayName="Tablo13" ref="A1:D14" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:D14" xr:uid="{47CC033D-BE82-E048-972C-A6CD74CE746C}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{BCEDA02B-B4FB-0946-9F40-8486D6856A6E}" name="Adjacency Matris Type" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{22890D4D-255E-4F47-864E-5CD826702D4E}" name="MSE" dataDxfId="9"/>
@@ -911,10 +917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9BF5BF4-2C7A-D644-B2C5-317E818EF65A}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1104,6 +1110,20 @@
       </c>
       <c r="D13" s="11" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="7">
+        <v>650</v>
+      </c>
+      <c r="C14" s="7">
+        <v>25.51</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1119,7 +1139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DD73E8-5331-DA4C-A46F-E23B3911B15E}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1137,68 +1157,68 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="33">
+      <c r="A2" s="29">
         <v>1963</v>
       </c>
-      <c r="B2" s="33">
+      <c r="B2" s="29">
         <v>44.31</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="29" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="33">
+      <c r="A3" s="29">
         <v>85</v>
       </c>
-      <c r="B3" s="33">
+      <c r="B3" s="29">
         <v>9.23</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="29" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="33">
+      <c r="A4" s="29">
         <v>77</v>
       </c>
-      <c r="B4" s="33">
+      <c r="B4" s="29">
         <v>8.8000000000000007</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="33">
+      <c r="A5" s="29">
         <v>259</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="29">
         <v>16.100000000000001</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="29" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="33">
+      <c r="A6" s="29">
         <v>243</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B6" s="29">
         <v>15.6</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="33">
+      <c r="A7" s="29">
         <v>222</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="29">
         <v>14.93</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="29" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1747,12 +1767,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
     </row>
     <row r="3" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
@@ -1797,12 +1817,12 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
     </row>
     <row r="7" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
@@ -1847,12 +1867,12 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
     </row>
     <row r="11" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
@@ -2001,36 +2021,36 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="31" t="s">
+      <c r="E2" s="31"/>
+      <c r="F2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31" t="s">
+      <c r="G2" s="32"/>
+      <c r="H2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="31"/>
+      <c r="I2" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">

</xml_diff>